<commit_message>
Clouds fixed, Mushrooms fixed, flowers fixed
</commit_message>
<xml_diff>
--- a/ShamanicSynesthesiaAssetList.xlsx
+++ b/ShamanicSynesthesiaAssetList.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/af89992d145862ba/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macuser/Documents/GitHub/Ancestral-Memories copy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="484" documentId="8_{16A3CED3-F267-7647-BDF9-6AF70DCC107C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{652F166F-75E7-0549-A56D-3E7E35818E23}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80186795-5678-374F-BDB8-50AE1B8B8F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2000" yWindow="0" windowWidth="35840" windowHeight="20480" xr2:uid="{5D038912-FC2F-F74B-A3CF-00147DC1AD42}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="99">
   <si>
     <t>Event Path</t>
   </si>
@@ -266,9 +266,6 @@
   </si>
   <si>
     <t>event:/UI/UI</t>
-  </si>
-  <si>
-    <t>event:/Weather/LightningStrike</t>
   </si>
   <si>
     <t>event:/Weather/Wind3D</t>
@@ -997,13 +994,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>116</xdr:row>
+      <xdr:row>115</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>673100</xdr:colOff>
-      <xdr:row>117</xdr:row>
+      <xdr:row>116</xdr:row>
       <xdr:rowOff>96308</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1349,10 +1346,10 @@
   <dimension ref="A1:CD149"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
-      <selection pane="bottomRight" activeCell="E44" sqref="E44"/>
+      <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1377,7 +1374,7 @@
     </row>
     <row r="2" spans="1:82" ht="51" x14ac:dyDescent="0.2">
       <c r="B2" s="40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -1411,7 +1408,7 @@
         <v>6</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:82" x14ac:dyDescent="0.2">
@@ -1436,14 +1433,14 @@
         <v>7</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G5" s="12"/>
       <c r="I5" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:82" ht="38" x14ac:dyDescent="0.2">
@@ -1458,14 +1455,14 @@
         <v>7</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G6" s="12"/>
       <c r="I6" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:82" s="10" customFormat="1" ht="20" x14ac:dyDescent="0.2">
@@ -1481,15 +1478,15 @@
         <v>7</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="23"/>
       <c r="J7" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
@@ -1578,7 +1575,7 @@
       <c r="G8" s="12"/>
       <c r="I8" s="23"/>
       <c r="J8" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:82" ht="20" x14ac:dyDescent="0.2">
@@ -1595,7 +1592,7 @@
       <c r="G9" s="12"/>
       <c r="I9" s="23"/>
       <c r="J9" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:82" ht="20" x14ac:dyDescent="0.2">
@@ -1610,14 +1607,14 @@
         <v>8</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I10" s="29"/>
       <c r="J10" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:82" ht="133" x14ac:dyDescent="0.2">
@@ -1626,14 +1623,14 @@
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
       <c r="F11" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="39" t="s">
         <v>84</v>
-      </c>
-      <c r="G11" s="39" t="s">
-        <v>85</v>
       </c>
       <c r="H11" s="28"/>
       <c r="I11" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:82" s="10" customFormat="1" ht="20" x14ac:dyDescent="0.2">
@@ -1668,11 +1665,11 @@
         <v>8</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I13" s="24"/>
       <c r="J13" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:82" x14ac:dyDescent="0.2">
@@ -1687,13 +1684,13 @@
         <v>8</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G14"/>
       <c r="H14"/>
       <c r="I14"/>
       <c r="J14" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:82" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -1708,13 +1705,13 @@
         <v>8</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G15"/>
       <c r="H15"/>
       <c r="I15"/>
       <c r="J15" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
@@ -1801,13 +1798,13 @@
         <v>7</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G16"/>
       <c r="H16"/>
       <c r="I16"/>
       <c r="J16" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
@@ -1893,13 +1890,13 @@
         <v>7</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G17"/>
       <c r="H17"/>
       <c r="I17"/>
       <c r="J17" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:81" ht="20" x14ac:dyDescent="0.2">
@@ -1914,13 +1911,13 @@
         <v>8</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G18"/>
       <c r="H18"/>
       <c r="I18"/>
       <c r="J18" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:81" s="10" customFormat="1" ht="20" x14ac:dyDescent="0.2">
@@ -1936,13 +1933,13 @@
         <v>8</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G19"/>
       <c r="H19"/>
       <c r="I19"/>
       <c r="J19" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
@@ -2028,15 +2025,15 @@
         <v>7</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G20"/>
       <c r="H20"/>
       <c r="I20" s="41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:81" ht="19" x14ac:dyDescent="0.25">
@@ -2051,13 +2048,13 @@
         <v>8</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G21" s="38"/>
       <c r="H21"/>
       <c r="I21"/>
       <c r="J21" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:81" x14ac:dyDescent="0.2">
@@ -2075,10 +2072,10 @@
       <c r="G22"/>
       <c r="H22"/>
       <c r="I22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:81" ht="20" x14ac:dyDescent="0.2">
@@ -2096,7 +2093,7 @@
       <c r="G23"/>
       <c r="H23"/>
       <c r="J23" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:81" ht="20" x14ac:dyDescent="0.2">
@@ -2111,13 +2108,13 @@
         <v>7</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G24"/>
       <c r="H24"/>
       <c r="I24"/>
       <c r="J24" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:81" ht="20" x14ac:dyDescent="0.2">
@@ -2136,7 +2133,7 @@
       <c r="H25"/>
       <c r="I25"/>
       <c r="J25" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:81" ht="20" x14ac:dyDescent="0.2">
@@ -2155,7 +2152,7 @@
       <c r="H26"/>
       <c r="I26"/>
       <c r="J26" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:81" ht="20" x14ac:dyDescent="0.2">
@@ -2174,7 +2171,7 @@
       <c r="H27"/>
       <c r="I27"/>
       <c r="J27" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:81" ht="20" x14ac:dyDescent="0.2">
@@ -2193,7 +2190,7 @@
       <c r="H28"/>
       <c r="I28"/>
       <c r="J28" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:81" s="21" customFormat="1" ht="20" x14ac:dyDescent="0.2">
@@ -2208,13 +2205,13 @@
         <v>7</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G29"/>
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K29" s="10"/>
       <c r="L29" s="10"/>
@@ -2300,15 +2297,15 @@
         <v>7</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H30"/>
       <c r="I30"/>
       <c r="J30" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:81" ht="95" x14ac:dyDescent="0.2">
@@ -2317,14 +2314,14 @@
       <c r="D31" s="28"/>
       <c r="E31" s="28"/>
       <c r="F31" s="39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G31" s="39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H31" s="28"/>
       <c r="I31" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:81" ht="20" x14ac:dyDescent="0.2">
@@ -2339,13 +2336,13 @@
         <v>8</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G32"/>
       <c r="H32"/>
       <c r="I32"/>
       <c r="J32" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:82" s="10" customFormat="1" ht="20" x14ac:dyDescent="0.2">
@@ -2365,7 +2362,7 @@
       <c r="H33"/>
       <c r="I33"/>
       <c r="J33" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K33" s="9"/>
       <c r="L33" s="9"/>
@@ -2457,7 +2454,7 @@
       <c r="H34"/>
       <c r="I34"/>
       <c r="J34" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K34" s="9"/>
       <c r="L34" s="9"/>
@@ -2549,7 +2546,7 @@
       <c r="H35"/>
       <c r="I35"/>
       <c r="J35" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K35" s="10" t="s">
         <v>9</v>
@@ -2612,8 +2609,8 @@
       <c r="D39" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E39" s="34" t="s">
-        <v>8</v>
+      <c r="E39" s="32" t="s">
+        <v>7</v>
       </c>
       <c r="F39"/>
       <c r="G39"/>
@@ -2693,21 +2690,17 @@
       <c r="CC39" s="9"/>
       <c r="CD39" s="9"/>
     </row>
-    <row r="40" spans="1:82" ht="20" x14ac:dyDescent="0.2">
-      <c r="B40" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="C40" s="35"/>
-      <c r="D40" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="F40"/>
-      <c r="G40"/>
-      <c r="H40"/>
-      <c r="I40"/>
+    <row r="40" spans="1:82" x14ac:dyDescent="0.2">
+      <c r="B40" s="42"/>
+      <c r="C40" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" s="44"/>
+      <c r="E40" s="44"/>
+      <c r="F40" s="44"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43"/>
       <c r="J40"/>
       <c r="K40"/>
       <c r="L40"/>
@@ -2774,9 +2767,7 @@
     <row r="41" spans="1:82" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="16"/>
       <c r="B41" s="42"/>
-      <c r="C41" s="45" t="s">
-        <v>99</v>
-      </c>
+      <c r="C41" s="44"/>
       <c r="D41" s="44"/>
       <c r="E41" s="44"/>
       <c r="F41" s="44"/>
@@ -2847,7 +2838,7 @@
       <c r="BS41"/>
     </row>
     <row r="42" spans="1:82" x14ac:dyDescent="0.2">
-      <c r="B42" s="42"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="44"/>
       <c r="D42" s="44"/>
       <c r="E42" s="44"/>
@@ -2920,14 +2911,14 @@
     </row>
     <row r="43" spans="1:82" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="16"/>
-      <c r="B43" s="43"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44"/>
-      <c r="F43" s="44"/>
-      <c r="G43" s="43"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
+      <c r="B43"/>
+      <c r="C43"/>
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43"/>
       <c r="J43" s="43"/>
       <c r="K43" s="43"/>
       <c r="L43" s="43"/>
@@ -6143,7 +6134,6 @@
     </row>
     <row r="86" spans="1:82" x14ac:dyDescent="0.2">
       <c r="B86"/>
-      <c r="C86"/>
       <c r="D86"/>
       <c r="E86"/>
       <c r="F86"/>
@@ -6234,30 +6224,39 @@
       <c r="CC87" s="9"/>
       <c r="CD87" s="9"/>
     </row>
-    <row r="88" spans="1:82" x14ac:dyDescent="0.2">
-      <c r="B88"/>
-      <c r="D88"/>
-      <c r="E88"/>
-      <c r="F88"/>
-      <c r="G88"/>
-      <c r="H88"/>
-      <c r="I88"/>
+    <row r="90" spans="1:82" x14ac:dyDescent="0.2">
+      <c r="D90" s="10"/>
+      <c r="E90" s="10"/>
+      <c r="F90" s="10"/>
+      <c r="G90" s="10"/>
+      <c r="H90" s="10"/>
+      <c r="I90" s="17"/>
     </row>
     <row r="91" spans="1:82" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="16"/>
       <c r="B91" s="9"/>
-      <c r="I91" s="17"/>
+      <c r="D91" s="9"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="12"/>
+      <c r="G91" s="9"/>
+      <c r="H91" s="9"/>
+      <c r="I91" s="20"/>
     </row>
     <row r="92" spans="1:82" x14ac:dyDescent="0.2">
-      <c r="F92" s="12"/>
+      <c r="B92" s="10"/>
     </row>
     <row r="93" spans="1:82" x14ac:dyDescent="0.2">
-      <c r="B93" s="10"/>
+      <c r="F93" s="12"/>
+      <c r="H93" s="12"/>
+      <c r="I93" s="9"/>
     </row>
     <row r="94" spans="1:82" x14ac:dyDescent="0.2">
-      <c r="F94" s="12"/>
-      <c r="H94" s="12"/>
-      <c r="I94" s="9"/>
+      <c r="D94" s="10"/>
+      <c r="E94" s="10"/>
+      <c r="F94" s="17"/>
+      <c r="G94" s="17"/>
+      <c r="H94" s="10"/>
+      <c r="I94" s="17"/>
     </row>
     <row r="95" spans="1:82" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="16"/>
@@ -6265,8 +6264,8 @@
       <c r="C95" s="10"/>
       <c r="D95" s="10"/>
       <c r="E95" s="10"/>
-      <c r="F95" s="17"/>
-      <c r="G95" s="17"/>
+      <c r="F95" s="10"/>
+      <c r="G95" s="10"/>
       <c r="H95" s="10"/>
       <c r="I95" s="17"/>
       <c r="J95" s="9"/>
@@ -6345,7 +6344,6 @@
     </row>
     <row r="96" spans="1:82" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="16"/>
-      <c r="B96" s="9"/>
       <c r="I96" s="17"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
@@ -6537,7 +6535,12 @@
     </row>
     <row r="140" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A140" s="16"/>
-      <c r="I140" s="17"/>
+      <c r="D140" s="9"/>
+      <c r="E140" s="9"/>
+      <c r="F140" s="9"/>
+      <c r="G140" s="9"/>
+      <c r="H140" s="9"/>
+      <c r="I140" s="20"/>
     </row>
     <row r="141" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A141" s="16"/>
@@ -6550,6 +6553,7 @@
     </row>
     <row r="142" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A142" s="16"/>
+      <c r="B142" s="9"/>
       <c r="D142" s="9"/>
       <c r="E142" s="9"/>
       <c r="F142" s="9"/>
@@ -6921,12 +6925,12 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D96:E96 D98:E1048576 E97 D11:E11 D1:E4">
+  <conditionalFormatting sqref="D95:E95 D97:E1048576 E96 D11:E11 D1:E4">
     <cfRule type="cellIs" dxfId="2" priority="11" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D89:E95">
+  <conditionalFormatting sqref="D88:E94">
     <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
       <formula>"Y"</formula>
     </cfRule>

</xml_diff>